<commit_message>
model and vol 26.02.18
</commit_message>
<xml_diff>
--- a/Data/Lab-linked/MESAlteckWater.xlsx
+++ b/Data/Lab-linked/MESAlteckWater.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>AO-W14-1</t>
   </si>
@@ -379,6 +379,15 @@
   </si>
   <si>
     <t>Conc.Solids.ug/gMES.SD</t>
+  </si>
+  <si>
+    <t>AFP-W16-1</t>
+  </si>
+  <si>
+    <t>AO-W16-1</t>
+  </si>
+  <si>
+    <t>W16-1</t>
   </si>
 </sst>
 </file>
@@ -804,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,7 +1872,9 @@
       <c r="D39" s="8">
         <v>50.00000000002558</v>
       </c>
-      <c r="E39" s="11"/>
+      <c r="E39" s="11">
+        <v>0</v>
+      </c>
       <c r="F39" s="1">
         <v>7.9999999999813554E-4</v>
       </c>
@@ -1875,6 +1886,26 @@
       </c>
       <c r="I39" s="2"/>
       <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="7">
+        <v>55</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>5.6000000000011596E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>